<commit_message>
optimized selection.py - should be the last time, hum ?
</commit_message>
<xml_diff>
--- a/sort/time_measurements.xlsx
+++ b/sort/time_measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTS\Cours ENJMIN\2022-09_Algorithmique et programmation\tp-python-algo-tri\sort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C5BF4B-CFE4-4A04-A4D5-ECE60F846BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2442BFB6-669C-476E-8CCC-F206EA4BD8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{CAEED006-1C04-4A08-8A68-4F0EFD1ED2F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CAEED006-1C04-4A08-8A68-4F0EFD1ED2F7}"/>
   </bookViews>
   <sheets>
     <sheet name="range" sheetId="1" r:id="rId1"/>
@@ -2360,7 +2360,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
completed tri par fusion
</commit_message>
<xml_diff>
--- a/sort/time_measurements.xlsx
+++ b/sort/time_measurements.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTS\Cours ENJMIN\2022-09_Algorithmique et programmation\tp-python-algo-tri\sort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2442BFB6-669C-476E-8CCC-F206EA4BD8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D491F737-14D6-4815-A8F6-6343276F33F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CAEED006-1C04-4A08-8A68-4F0EFD1ED2F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CAEED006-1C04-4A08-8A68-4F0EFD1ED2F7}"/>
   </bookViews>
   <sheets>
     <sheet name="range" sheetId="1" r:id="rId1"/>
-    <sheet name="selection" sheetId="3" r:id="rId2"/>
+    <sheet name="selection" sheetId="4" r:id="rId2"/>
+    <sheet name="insertion" sheetId="3" r:id="rId3"/>
+    <sheet name="fusion" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>Array size</t>
   </si>
@@ -587,7 +589,657 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EAF6-40C7-8D9A-15B5CFD62F66}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1043923504"/>
+        <c:axId val="1043923920"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1043923504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1043923920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1043923920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000000000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1043923504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>insertion!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>insertion!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>insertion!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.110998630523681</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70382499694824197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1400225162506099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8597722053527797</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2124927043914795</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.494237422943099</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.421517372131301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.4183061122894</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.3886976242065</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70.410352706909094</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-21D9-419D-94B0-B9725C0B447C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1043923504"/>
+        <c:axId val="1043923920"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1043923504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1043923920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1043923920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000000000000000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1043923504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fusion!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>fusion!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fusion!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000000000000000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3.0269622802734301E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0193748474121094E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.50110721588134E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7029523849487301E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.09982395172119E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5034666061401301E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1642198562622001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.9030790328979402E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.1033983230590799E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0997495651245103E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-747D-4D18-A19E-BD00F823ECD6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -835,6 +1487,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1352,6 +2084,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1928,7 +3692,93 @@
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41F3000D-773B-4550-A1A4-5724011155D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D5E9A9C-285D-4529-AA98-BA77EF1294C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>655320</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15C8E582-1A19-44AE-89DF-9280F2111386}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2356,10 +4206,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8878299C-3157-4348-B8B9-0D5F04F10B80}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C3D174-ABCF-4183-821D-65576344D4E3}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
@@ -2462,4 +4312,222 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8878299C-3157-4348-B8B9-0D5F04F10B80}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="22.77734375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.110998630523681</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.70382499694824197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.1400225162506099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4.8597722053527797</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9.2124927043914795</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6000</v>
+      </c>
+      <c r="B7" s="2">
+        <v>15.494237422943099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7000</v>
+      </c>
+      <c r="B8" s="2">
+        <v>24.421517372131301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B9" s="2">
+        <v>36.4183061122894</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9000</v>
+      </c>
+      <c r="B10" s="2">
+        <v>52.3886976242065</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B11" s="2">
+        <v>70.410352706909094</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465253BF-5C92-49DA-A14E-2F30E0A56F8B}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="22.77734375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3.0269622802734301E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9.0193748474121094E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3000</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.50110721588134E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.7029523849487301E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.09982395172119E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6000</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.5034666061401301E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7000</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.1642198562622001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8000</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.9030790328979402E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9000</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4.1033983230590799E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5.0997495651245103E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>